<commit_message>
Deleted files : trash.py
</commit_message>
<xml_diff>
--- a/file1.xlsx
+++ b/file1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Pythonproject/ProjetSynthese/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA61CA2E-48B7-B847-93E7-7B5621016154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D26981C-3379-CB48-94C4-D658D32AADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>s</t>
   </si>
@@ -384,15 +384,15 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="B1">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
@@ -400,16 +400,16 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
+      <c r="B3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
+      <c r="B4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>